<commit_message>
old excel sheet format
</commit_message>
<xml_diff>
--- a/notes/fertilization/fertilizer_addition_20240607.xlsx
+++ b/notes/fertilization/fertilizer_addition_20240607.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/fertilization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/notes/fertilization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC2FCF4-D37D-CE45-870E-A93D829A2451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A131AB-94AB-0442-97E9-37B976028201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{894E8D85-BD71-D744-B56B-250ABA74CB59}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>